<commit_message>
first attempt at EDA
sadly unsurprising (but still monumental) results
</commit_message>
<xml_diff>
--- a/2019-sqf-file-spec.xlsx
+++ b/2019-sqf-file-spec.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10510"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3208E3EE-2537-D349-A74A-F1F7512753E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D74A383-E06B-294E-8392-571B43667165}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="460" windowWidth="25600" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19980" yWindow="1440" windowWidth="28120" windowHeight="18800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stop Report Index" sheetId="1" r:id="rId1"/>
@@ -881,18 +881,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -949,6 +937,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1528,7 +1528,7 @@
       <c r="C30" t="s">
         <v>187</v>
       </c>
-      <c r="D30" s="11" t="s">
+      <c r="D30" s="30" t="s">
         <v>186</v>
       </c>
     </row>
@@ -1542,7 +1542,7 @@
       <c r="C31" t="s">
         <v>187</v>
       </c>
-      <c r="D31" s="12"/>
+      <c r="D31" s="31"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="9" t="s">
@@ -1554,7 +1554,7 @@
       <c r="C32" t="s">
         <v>187</v>
       </c>
-      <c r="D32" s="12"/>
+      <c r="D32" s="31"/>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="9" t="s">
@@ -1566,7 +1566,7 @@
       <c r="C33" t="s">
         <v>187</v>
       </c>
-      <c r="D33" s="13"/>
+      <c r="D33" s="32"/>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="9" t="s">
@@ -1578,7 +1578,7 @@
       <c r="C34" t="s">
         <v>187</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="D34" s="33" t="s">
         <v>188</v>
       </c>
     </row>
@@ -1592,7 +1592,7 @@
       <c r="C35" t="s">
         <v>187</v>
       </c>
-      <c r="D35" s="13"/>
+      <c r="D35" s="32"/>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="9" t="s">
@@ -2162,8 +2162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C75A25E-286D-D247-89B4-3CDFEF7DEFC2}">
   <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2174,856 +2174,856 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="14" t="s">
         <v>194</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="15" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="32">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="16" t="s">
         <v>223</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:4" ht="16">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
     </row>
     <row r="4" spans="1:4" ht="16">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16" t="s">
+      <c r="C4" s="12"/>
+      <c r="D4" s="12" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
     </row>
     <row r="6" spans="1:4" ht="16">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
     </row>
     <row r="7" spans="1:4" ht="16">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
     </row>
     <row r="8" spans="1:4" ht="48">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="D8" s="16"/>
+      <c r="D8" s="12"/>
     </row>
     <row r="9" spans="1:4" ht="16">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="29" t="s">
         <v>203</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="29" t="s">
         <v>207</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="29" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="32">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="12" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="12" t="s">
         <v>209</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="12" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="32">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="12" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="12" t="s">
         <v>209</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="12" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="12" t="s">
         <v>213</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="12" t="s">
         <v>212</v>
       </c>
-      <c r="D14" s="16"/>
+      <c r="D14" s="12"/>
     </row>
     <row r="15" spans="1:4" ht="16">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="D15" s="16"/>
+      <c r="D15" s="12"/>
     </row>
     <row r="16" spans="1:4" ht="16">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="D16" s="16"/>
+      <c r="D16" s="12"/>
     </row>
     <row r="17" spans="1:4" ht="16">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="D17" s="16"/>
+      <c r="D17" s="12"/>
     </row>
     <row r="18" spans="1:4" ht="32">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="12" t="s">
         <v>218</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="D18" s="16"/>
+      <c r="D18" s="12"/>
     </row>
     <row r="19" spans="1:4" ht="32">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23" t="s">
+      <c r="C19" s="19"/>
+      <c r="D19" s="19" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="16">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="33"/>
-      <c r="C20" s="33" t="s">
-        <v>187</v>
-      </c>
-      <c r="D20" s="33"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29" t="s">
+        <v>187</v>
+      </c>
+      <c r="D20" s="29"/>
     </row>
     <row r="21" spans="1:4" ht="16">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="28" t="s">
-        <v>187</v>
-      </c>
-      <c r="D21" s="28"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="D21" s="24"/>
     </row>
     <row r="22" spans="1:4" ht="16">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="21" t="s">
         <v>222</v>
       </c>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23" t="s">
+      <c r="C22" s="19"/>
+      <c r="D22" s="19" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="16">
-      <c r="A23" s="32" t="s">
+      <c r="A23" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="33"/>
-      <c r="C23" s="33" t="s">
-        <v>187</v>
-      </c>
-      <c r="D23" s="33"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29" t="s">
+        <v>187</v>
+      </c>
+      <c r="D23" s="29"/>
     </row>
     <row r="24" spans="1:4" ht="32">
-      <c r="A24" s="32" t="s">
+      <c r="A24" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33" t="s">
+      <c r="B24" s="29"/>
+      <c r="C24" s="29" t="s">
         <v>221</v>
       </c>
-      <c r="D24" s="33"/>
+      <c r="D24" s="29"/>
     </row>
     <row r="25" spans="1:4" ht="64">
-      <c r="A25" s="30" t="s">
+      <c r="A25" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="D25" s="15" t="s">
+      <c r="B25" s="12"/>
+      <c r="C25" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D25" s="11" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="16">
-      <c r="A26" s="30" t="s">
+      <c r="A26" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="16"/>
-      <c r="C26" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="D26" s="15"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D26" s="11"/>
     </row>
     <row r="27" spans="1:4" ht="16">
-      <c r="A27" s="30" t="s">
+      <c r="A27" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="D27" s="15"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D27" s="11"/>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1">
-      <c r="A28" s="30" t="s">
+      <c r="A28" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="D28" s="15"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D28" s="11"/>
     </row>
     <row r="29" spans="1:4" ht="16">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="D29" s="15" t="s">
+      <c r="B29" s="12"/>
+      <c r="C29" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D29" s="11" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="16">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="D30" s="15"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D30" s="11"/>
     </row>
     <row r="31" spans="1:4" ht="16">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="16"/>
-      <c r="C31" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="D31" s="16" t="s">
+      <c r="B31" s="12"/>
+      <c r="C31" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D31" s="12" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="16">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="16"/>
-      <c r="C32" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="D32" s="16"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D32" s="12"/>
     </row>
     <row r="33" spans="1:4" ht="16">
-      <c r="A33" s="31" t="s">
+      <c r="A33" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="16"/>
-      <c r="C33" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="D33" s="16"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D33" s="12"/>
     </row>
     <row r="34" spans="1:4" ht="16">
-      <c r="A34" s="31" t="s">
+      <c r="A34" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="16"/>
-      <c r="C34" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="D34" s="16"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D34" s="12"/>
     </row>
     <row r="35" spans="1:4" ht="16">
-      <c r="A35" s="31" t="s">
+      <c r="A35" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="16"/>
-      <c r="C35" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="D35" s="16"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D35" s="12"/>
     </row>
     <row r="36" spans="1:4" ht="16">
-      <c r="A36" s="31" t="s">
+      <c r="A36" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="16"/>
-      <c r="C36" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="D36" s="16"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D36" s="12"/>
     </row>
     <row r="37" spans="1:4" ht="16">
-      <c r="A37" s="31" t="s">
+      <c r="A37" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="B37" s="16"/>
-      <c r="C37" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="D37" s="16"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D37" s="12"/>
     </row>
     <row r="38" spans="1:4" ht="16">
-      <c r="A38" s="26" t="s">
+      <c r="A38" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="16"/>
-      <c r="C38" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="D38" s="16"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D38" s="12"/>
     </row>
     <row r="39" spans="1:4" ht="16">
-      <c r="A39" s="26" t="s">
+      <c r="A39" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="16"/>
-      <c r="C39" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="D39" s="16"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D39" s="12"/>
     </row>
     <row r="40" spans="1:4" ht="16">
-      <c r="A40" s="26" t="s">
+      <c r="A40" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="B40" s="16"/>
-      <c r="C40" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="D40" s="16"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D40" s="12"/>
     </row>
     <row r="41" spans="1:4" ht="16">
-      <c r="A41" s="26" t="s">
+      <c r="A41" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="B41" s="16"/>
-      <c r="C41" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="D41" s="16"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D41" s="12"/>
     </row>
     <row r="42" spans="1:4" ht="16">
-      <c r="A42" s="26" t="s">
+      <c r="A42" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="16"/>
-      <c r="C42" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="D42" s="16"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D42" s="12"/>
     </row>
     <row r="43" spans="1:4" ht="16">
-      <c r="A43" s="26" t="s">
+      <c r="A43" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="16"/>
-      <c r="C43" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="D43" s="16"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D43" s="12"/>
     </row>
     <row r="44" spans="1:4" ht="16">
-      <c r="A44" s="26" t="s">
+      <c r="A44" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="16"/>
-      <c r="C44" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="D44" s="16"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D44" s="12"/>
     </row>
     <row r="45" spans="1:4" ht="16">
-      <c r="A45" s="26" t="s">
+      <c r="A45" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="16"/>
-      <c r="C45" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="D45" s="16"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D45" s="12"/>
     </row>
     <row r="46" spans="1:4" ht="16">
-      <c r="A46" s="26" t="s">
+      <c r="A46" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="B46" s="16"/>
-      <c r="C46" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="D46" s="16"/>
+      <c r="B46" s="12"/>
+      <c r="C46" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D46" s="12"/>
     </row>
     <row r="47" spans="1:4" ht="16">
-      <c r="A47" s="26" t="s">
+      <c r="A47" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="B47" s="16"/>
-      <c r="C47" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="D47" s="16"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D47" s="12"/>
     </row>
     <row r="48" spans="1:4" ht="16">
-      <c r="A48" s="31" t="s">
+      <c r="A48" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="B48" s="16"/>
-      <c r="C48" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="D48" s="16"/>
+      <c r="B48" s="12"/>
+      <c r="C48" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D48" s="12"/>
     </row>
     <row r="49" spans="1:4" ht="16">
-      <c r="A49" s="31" t="s">
+      <c r="A49" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="B49" s="16"/>
-      <c r="C49" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="D49" s="16"/>
+      <c r="B49" s="12"/>
+      <c r="C49" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D49" s="12"/>
     </row>
     <row r="50" spans="1:4" ht="16">
-      <c r="A50" s="31" t="s">
+      <c r="A50" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="B50" s="16"/>
-      <c r="C50" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="D50" s="16"/>
+      <c r="B50" s="12"/>
+      <c r="C50" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D50" s="12"/>
     </row>
     <row r="51" spans="1:4" ht="16">
-      <c r="A51" s="31" t="s">
+      <c r="A51" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="B51" s="16"/>
-      <c r="C51" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="D51" s="16"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D51" s="12"/>
     </row>
     <row r="52" spans="1:4" ht="16">
-      <c r="A52" s="31" t="s">
+      <c r="A52" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="B52" s="16"/>
-      <c r="C52" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="D52" s="16"/>
+      <c r="B52" s="12"/>
+      <c r="C52" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D52" s="12"/>
     </row>
     <row r="53" spans="1:4" ht="16">
-      <c r="A53" s="31" t="s">
+      <c r="A53" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="B53" s="16"/>
-      <c r="C53" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="D53" s="16"/>
+      <c r="B53" s="12"/>
+      <c r="C53" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D53" s="12"/>
     </row>
     <row r="54" spans="1:4" ht="16">
-      <c r="A54" s="31" t="s">
+      <c r="A54" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="B54" s="16"/>
-      <c r="C54" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="D54" s="16"/>
+      <c r="B54" s="12"/>
+      <c r="C54" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D54" s="12"/>
     </row>
     <row r="55" spans="1:4" ht="16">
-      <c r="A55" s="31" t="s">
+      <c r="A55" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="B55" s="16"/>
-      <c r="C55" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="D55" s="16"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D55" s="12"/>
     </row>
     <row r="56" spans="1:4" ht="16">
-      <c r="A56" s="26" t="s">
+      <c r="A56" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B56" s="16"/>
-      <c r="C56" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="D56" s="16"/>
+      <c r="B56" s="12"/>
+      <c r="C56" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D56" s="12"/>
     </row>
     <row r="57" spans="1:4" ht="16">
-      <c r="A57" s="26" t="s">
+      <c r="A57" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="B57" s="16"/>
-      <c r="C57" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="D57" s="16"/>
+      <c r="B57" s="12"/>
+      <c r="C57" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D57" s="12"/>
     </row>
     <row r="58" spans="1:4" ht="16">
-      <c r="A58" s="26" t="s">
+      <c r="A58" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B58" s="16"/>
-      <c r="C58" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="D58" s="16"/>
+      <c r="B58" s="12"/>
+      <c r="C58" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D58" s="12"/>
     </row>
     <row r="59" spans="1:4" ht="16">
-      <c r="A59" s="26" t="s">
+      <c r="A59" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="B59" s="16"/>
-      <c r="C59" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="D59" s="16"/>
+      <c r="B59" s="12"/>
+      <c r="C59" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D59" s="12"/>
     </row>
     <row r="60" spans="1:4" ht="16">
-      <c r="A60" s="26" t="s">
+      <c r="A60" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="B60" s="16"/>
-      <c r="C60" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="D60" s="16"/>
+      <c r="B60" s="12"/>
+      <c r="C60" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D60" s="12"/>
     </row>
     <row r="61" spans="1:4" ht="16">
-      <c r="A61" s="26" t="s">
+      <c r="A61" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="B61" s="16"/>
-      <c r="C61" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="D61" s="16"/>
+      <c r="B61" s="12"/>
+      <c r="C61" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D61" s="12"/>
     </row>
     <row r="62" spans="1:4" ht="16">
-      <c r="A62" s="26" t="s">
+      <c r="A62" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="B62" s="16"/>
-      <c r="C62" s="16"/>
-      <c r="D62" s="16"/>
+      <c r="B62" s="12"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="12"/>
     </row>
     <row r="63" spans="1:4" ht="48">
-      <c r="A63" s="22" t="s">
+      <c r="A63" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B63" s="23"/>
-      <c r="C63" s="24" t="s">
+      <c r="B63" s="19"/>
+      <c r="C63" s="20" t="s">
         <v>192</v>
       </c>
-      <c r="D63" s="23" t="s">
+      <c r="D63" s="19" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="16">
-      <c r="A64" s="31" t="s">
+      <c r="A64" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="B64" s="16"/>
-      <c r="C64" s="16"/>
-      <c r="D64" s="16" t="s">
+      <c r="B64" s="12"/>
+      <c r="C64" s="12"/>
+      <c r="D64" s="12" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="16">
-      <c r="A65" s="31" t="s">
+      <c r="A65" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="B65" s="16"/>
-      <c r="C65" s="16" t="s">
+      <c r="B65" s="12"/>
+      <c r="C65" s="12" t="s">
         <v>191</v>
       </c>
-      <c r="D65" s="16" t="s">
+      <c r="D65" s="12" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="16">
-      <c r="A66" s="31" t="s">
+      <c r="A66" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="B66" s="16"/>
-      <c r="C66" s="16"/>
-      <c r="D66" s="16" t="s">
+      <c r="B66" s="12"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="12" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="16">
-      <c r="A67" s="31" t="s">
+      <c r="A67" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="B67" s="16"/>
-      <c r="C67" s="16"/>
-      <c r="D67" s="16" t="s">
+      <c r="B67" s="12"/>
+      <c r="C67" s="12"/>
+      <c r="D67" s="12" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="16">
-      <c r="A68" s="31" t="s">
+      <c r="A68" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="B68" s="16"/>
-      <c r="C68" s="16"/>
-      <c r="D68" s="16" t="s">
+      <c r="B68" s="12"/>
+      <c r="C68" s="12"/>
+      <c r="D68" s="12" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="16">
-      <c r="A69" s="31" t="s">
+      <c r="A69" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="B69" s="16"/>
-      <c r="C69" s="16"/>
-      <c r="D69" s="16" t="s">
+      <c r="B69" s="12"/>
+      <c r="C69" s="12"/>
+      <c r="D69" s="12" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="16">
-      <c r="A70" s="31" t="s">
+      <c r="A70" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="B70" s="16"/>
-      <c r="C70" s="16"/>
-      <c r="D70" s="16" t="s">
+      <c r="B70" s="12"/>
+      <c r="C70" s="12"/>
+      <c r="D70" s="12" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="16">
-      <c r="A71" s="31" t="s">
+      <c r="A71" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="B71" s="16"/>
-      <c r="C71" s="16"/>
-      <c r="D71" s="16" t="s">
+      <c r="B71" s="12"/>
+      <c r="C71" s="12"/>
+      <c r="D71" s="12" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="48">
-      <c r="A72" s="22" t="s">
+      <c r="A72" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="B72" s="23"/>
-      <c r="C72" s="24" t="s">
+      <c r="B72" s="19"/>
+      <c r="C72" s="20" t="s">
         <v>192</v>
       </c>
-      <c r="D72" s="23" t="s">
+      <c r="D72" s="19" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="16">
-      <c r="A73" s="29" t="s">
+      <c r="A73" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="B73" s="16"/>
-      <c r="C73" s="16"/>
-      <c r="D73" s="16"/>
+      <c r="B73" s="12"/>
+      <c r="C73" s="12"/>
+      <c r="D73" s="12"/>
     </row>
     <row r="74" spans="1:4" ht="16">
-      <c r="A74" s="29" t="s">
+      <c r="A74" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="B74" s="16"/>
-      <c r="C74" s="16"/>
-      <c r="D74" s="16"/>
+      <c r="B74" s="12"/>
+      <c r="C74" s="12"/>
+      <c r="D74" s="12"/>
     </row>
     <row r="75" spans="1:4" ht="16">
-      <c r="A75" s="29" t="s">
+      <c r="A75" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="B75" s="16"/>
-      <c r="C75" s="16"/>
-      <c r="D75" s="16"/>
+      <c r="B75" s="12"/>
+      <c r="C75" s="12"/>
+      <c r="D75" s="12"/>
     </row>
     <row r="76" spans="1:4" ht="16">
-      <c r="A76" s="29" t="s">
+      <c r="A76" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="B76" s="16"/>
-      <c r="C76" s="16"/>
-      <c r="D76" s="16"/>
+      <c r="B76" s="12"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
     </row>
     <row r="77" spans="1:4" ht="16">
-      <c r="A77" s="29" t="s">
+      <c r="A77" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="B77" s="16"/>
-      <c r="C77" s="16"/>
-      <c r="D77" s="16"/>
+      <c r="B77" s="12"/>
+      <c r="C77" s="12"/>
+      <c r="D77" s="12"/>
     </row>
     <row r="78" spans="1:4" ht="16">
-      <c r="A78" s="29" t="s">
+      <c r="A78" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="B78" s="16"/>
-      <c r="C78" s="16"/>
-      <c r="D78" s="16"/>
+      <c r="B78" s="12"/>
+      <c r="C78" s="12"/>
+      <c r="D78" s="12"/>
     </row>
     <row r="79" spans="1:4" ht="16">
-      <c r="A79" s="29" t="s">
+      <c r="A79" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="B79" s="16"/>
-      <c r="C79" s="16"/>
-      <c r="D79" s="16"/>
+      <c r="B79" s="12"/>
+      <c r="C79" s="12"/>
+      <c r="D79" s="12"/>
     </row>
     <row r="80" spans="1:4" ht="16">
-      <c r="A80" s="29" t="s">
+      <c r="A80" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="B80" s="16"/>
-      <c r="C80" s="16"/>
-      <c r="D80" s="16"/>
+      <c r="B80" s="12"/>
+      <c r="C80" s="12"/>
+      <c r="D80" s="12"/>
     </row>
     <row r="81" spans="1:4" ht="16">
-      <c r="A81" s="29" t="s">
+      <c r="A81" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="B81" s="16"/>
-      <c r="C81" s="16"/>
-      <c r="D81" s="16"/>
+      <c r="B81" s="12"/>
+      <c r="C81" s="12"/>
+      <c r="D81" s="12"/>
     </row>
     <row r="82" spans="1:4" ht="16">
-      <c r="A82" s="29" t="s">
+      <c r="A82" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="B82" s="16"/>
-      <c r="C82" s="16"/>
-      <c r="D82" s="16"/>
+      <c r="B82" s="12"/>
+      <c r="C82" s="12"/>
+      <c r="D82" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>